<commit_message>
add common info editor
</commit_message>
<xml_diff>
--- a/plugin/act_builder_lib/actOSR.xlsx
+++ b/plugin/act_builder_lib/actOSR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danek\Documents\GitHub\builders_act_maker\c#\ActBuilder\bin\Debug\net6.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danek\Documents\GitHub\builders_act_maker\plugin\act_builder_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C42145E2-386E-40B1-9FBA-5A7CB1F29577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2461E27-AFD4-42D6-9C93-F7E8BD741F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
@@ -392,14 +392,6 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -726,13 +718,13 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -771,17 +763,62 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -798,9 +835,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -810,62 +844,17 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="12" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="12" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1253,8 +1242,8 @@
   </sheetPr>
   <dimension ref="A1:BE88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A65" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A87" sqref="A87:J87"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1276,12 +1265,12 @@
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
@@ -1296,98 +1285,98 @@
       <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
     </row>
     <row r="4" spans="1:10" s="11" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
     </row>
     <row r="6" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
     </row>
     <row r="8" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="37"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
     </row>
     <row r="9" spans="1:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
@@ -1398,97 +1387,97 @@
       <c r="D10" s="17"/>
       <c r="E10" s="17"/>
       <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
     </row>
     <row r="14" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
     </row>
     <row r="15" spans="1:10" s="11" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36"/>
+      <c r="E15" s="36"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="36"/>
+      <c r="J15" s="36"/>
     </row>
     <row r="16" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
     </row>
     <row r="17" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B17" s="7"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
     </row>
     <row r="18" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1513,11 +1502,11 @@
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
       <c r="E20" s="15"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
+      <c r="J20" s="33"/>
     </row>
     <row r="21" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
@@ -1532,18 +1521,18 @@
       <c r="J21" s="15"/>
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
     </row>
     <row r="23" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
@@ -1560,30 +1549,30 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B25" s="19"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
     </row>
     <row r="26" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
@@ -1613,18 +1602,18 @@
       <c r="J27" s="15"/>
     </row>
     <row r="28" spans="1:12" s="4" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
@@ -1642,30 +1631,30 @@
       <c r="L29" s="10"/>
     </row>
     <row r="30" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
     </row>
     <row r="31" spans="1:12" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
     </row>
     <row r="32" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
@@ -1679,33 +1668,33 @@
       <c r="G32" s="17"/>
       <c r="H32" s="17"/>
       <c r="I32" s="15"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="33"/>
     </row>
     <row r="33" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
+      <c r="A33" s="34"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
     </row>
     <row r="34" spans="1:57" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
     </row>
     <row r="35" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
@@ -1722,30 +1711,30 @@
       <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
     </row>
     <row r="37" spans="1:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="33" t="s">
+      <c r="A37" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="33"/>
-      <c r="C37" s="33"/>
-      <c r="D37" s="33"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
-      <c r="G37" s="33"/>
-      <c r="H37" s="33"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="33"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="25"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
     </row>
     <row r="38" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
@@ -1766,14 +1755,14 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
-      <c r="I39" s="35"/>
-      <c r="J39" s="35"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
     </row>
     <row r="40" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
@@ -1799,30 +1788,30 @@
       <c r="J41" s="15"/>
     </row>
     <row r="42" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="A42" s="30"/>
+      <c r="B42" s="30"/>
+      <c r="C42" s="30"/>
+      <c r="D42" s="30"/>
+      <c r="E42" s="30"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
+      <c r="J42" s="30"/>
     </row>
     <row r="43" spans="1:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="33" t="s">
+      <c r="A43" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="33"/>
-      <c r="C43" s="33"/>
-      <c r="D43" s="33"/>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
     </row>
     <row r="44" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
@@ -1851,18 +1840,18 @@
       <c r="J45" s="15"/>
     </row>
     <row r="46" spans="1:57" s="4" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="34"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="28"/>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
     </row>
     <row r="47" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
@@ -1871,24 +1860,24 @@
       <c r="B47" s="17"/>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="18"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+      <c r="J47" s="20"/>
     </row>
     <row r="48" spans="1:57" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="41"/>
+      <c r="A48" s="44"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="45"/>
+      <c r="H48" s="45"/>
+      <c r="I48" s="45"/>
+      <c r="J48" s="45"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
@@ -1938,18 +1927,18 @@
       <c r="BE48" s="6"/>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="33" t="s">
+      <c r="A49" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="33"/>
-      <c r="C49" s="33"/>
-      <c r="D49" s="33"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="33"/>
-      <c r="G49" s="33"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="33"/>
-      <c r="J49" s="33"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
     </row>
     <row r="50" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
@@ -1966,42 +1955,42 @@
       <c r="J50" s="17"/>
     </row>
     <row r="51" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="42"/>
-      <c r="B51" s="43"/>
-      <c r="C51" s="43"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="43"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="43"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="43"/>
-      <c r="J51" s="43"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="46"/>
+      <c r="D51" s="46"/>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
+      <c r="J51" s="46"/>
     </row>
     <row r="52" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="B52" s="19"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="19"/>
-      <c r="E52" s="19"/>
-      <c r="F52" s="19"/>
-      <c r="G52" s="19"/>
-      <c r="H52" s="19"/>
-      <c r="I52" s="19"/>
-      <c r="J52" s="19"/>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="16"/>
+      <c r="J52" s="16"/>
     </row>
     <row r="53" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="37"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="23"/>
+      <c r="C53" s="23"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
     </row>
     <row r="54" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
@@ -2011,10 +2000,10 @@
         <v>12</v>
       </c>
       <c r="D54" s="13"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
     </row>
     <row r="55" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D55" s="2"/>
@@ -2026,22 +2015,22 @@
         <v>13</v>
       </c>
       <c r="D56" s="13"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
+      <c r="E56" s="27"/>
+      <c r="F56" s="27"/>
+      <c r="G56" s="27"/>
+      <c r="H56" s="27"/>
     </row>
     <row r="57" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="38"/>
-      <c r="B57" s="38"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="38"/>
-      <c r="E57" s="38"/>
-      <c r="F57" s="38"/>
-      <c r="G57" s="38"/>
-      <c r="H57" s="38"/>
-      <c r="I57" s="38"/>
-      <c r="J57" s="38"/>
+      <c r="A57" s="18"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="18"/>
+      <c r="D57" s="18"/>
+      <c r="E57" s="18"/>
+      <c r="F57" s="18"/>
+      <c r="G57" s="18"/>
+      <c r="H57" s="18"/>
+      <c r="I57" s="18"/>
+      <c r="J57" s="18"/>
     </row>
     <row r="58" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
@@ -2051,37 +2040,37 @@
       <c r="C58" s="17"/>
       <c r="D58" s="17"/>
       <c r="E58" s="15"/>
-      <c r="F58" s="39"/>
-      <c r="G58" s="39"/>
-      <c r="H58" s="39"/>
-      <c r="I58" s="39"/>
-      <c r="J58" s="39"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+      <c r="I58" s="24"/>
+      <c r="J58" s="24"/>
     </row>
     <row r="59" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="30"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
-      <c r="F59" s="30"/>
-      <c r="G59" s="30"/>
-      <c r="H59" s="30"/>
-      <c r="I59" s="30"/>
-      <c r="J59" s="30"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="26"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="26"/>
+      <c r="E59" s="26"/>
+      <c r="F59" s="26"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="26"/>
+      <c r="I59" s="26"/>
+      <c r="J59" s="26"/>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="B60" s="19"/>
-      <c r="C60" s="19"/>
-      <c r="D60" s="19"/>
-      <c r="E60" s="19"/>
-      <c r="F60" s="19"/>
-      <c r="G60" s="19"/>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="19"/>
+      <c r="B60" s="16"/>
+      <c r="C60" s="16"/>
+      <c r="D60" s="16"/>
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="16"/>
+      <c r="J60" s="16"/>
     </row>
     <row r="61" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
@@ -2110,18 +2099,18 @@
       <c r="J62" s="15"/>
     </row>
     <row r="63" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+      <c r="A63" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="19"/>
-      <c r="C63" s="19"/>
-      <c r="D63" s="19"/>
-      <c r="E63" s="19"/>
-      <c r="F63" s="19"/>
-      <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="19"/>
+      <c r="B63" s="16"/>
+      <c r="C63" s="16"/>
+      <c r="D63" s="16"/>
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="16"/>
+      <c r="J63" s="16"/>
     </row>
     <row r="64" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
@@ -2139,12 +2128,12 @@
     </row>
     <row r="65" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="47" t="s">
+      <c r="A66" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B66" s="47"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19"/>
     </row>
     <row r="67" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
@@ -2173,18 +2162,18 @@
       <c r="J68" s="15"/>
     </row>
     <row r="69" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
+      <c r="D69" s="16"/>
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="16"/>
+      <c r="H69" s="16"/>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
     </row>
     <row r="70" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
@@ -2207,12 +2196,12 @@
       <c r="B71" s="17"/>
       <c r="C71" s="17"/>
       <c r="D71" s="17"/>
-      <c r="E71" s="38"/>
-      <c r="F71" s="38"/>
-      <c r="G71" s="38"/>
-      <c r="H71" s="38"/>
-      <c r="I71" s="38"/>
-      <c r="J71" s="38"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="18"/>
+      <c r="G71" s="18"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="18"/>
+      <c r="J71" s="18"/>
     </row>
     <row r="72" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
@@ -2227,18 +2216,18 @@
       <c r="J72" s="15"/>
     </row>
     <row r="73" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="19"/>
-      <c r="E73" s="19"/>
-      <c r="F73" s="19"/>
-      <c r="G73" s="19"/>
-      <c r="H73" s="19"/>
-      <c r="I73" s="19"/>
-      <c r="J73" s="19"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16"/>
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="16"/>
+      <c r="I73" s="16"/>
+      <c r="J73" s="16"/>
     </row>
     <row r="74" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
@@ -2248,11 +2237,11 @@
       <c r="C74" s="17"/>
       <c r="D74" s="17"/>
       <c r="E74" s="17"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
-      <c r="I74" s="18"/>
-      <c r="J74" s="18"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
+      <c r="I74" s="20"/>
+      <c r="J74" s="20"/>
       <c r="L74" s="10"/>
     </row>
     <row r="75" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2268,18 +2257,18 @@
       <c r="J75" s="15"/>
     </row>
     <row r="76" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19"/>
-      <c r="F76" s="19"/>
-      <c r="G76" s="19"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-      <c r="J76" s="19"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="16"/>
+      <c r="D76" s="16"/>
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="16"/>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+      <c r="J76" s="16"/>
     </row>
     <row r="77" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
@@ -2309,18 +2298,18 @@
       <c r="J78" s="15"/>
     </row>
     <row r="79" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B79" s="19"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="19"/>
-      <c r="E79" s="19"/>
-      <c r="F79" s="19"/>
-      <c r="G79" s="19"/>
-      <c r="H79" s="19"/>
-      <c r="I79" s="19"/>
-      <c r="J79" s="19"/>
+      <c r="B79" s="16"/>
+      <c r="C79" s="16"/>
+      <c r="D79" s="16"/>
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="16"/>
+      <c r="H79" s="16"/>
+      <c r="I79" s="16"/>
+      <c r="J79" s="16"/>
     </row>
     <row r="80" spans="1:12" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
@@ -2333,8 +2322,8 @@
       <c r="F80" s="17"/>
       <c r="G80" s="17"/>
       <c r="H80" s="17"/>
-      <c r="I80" s="18"/>
-      <c r="J80" s="18"/>
+      <c r="I80" s="20"/>
+      <c r="J80" s="20"/>
     </row>
     <row r="81" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="15"/>
@@ -2345,22 +2334,22 @@
       <c r="F81" s="15"/>
       <c r="G81" s="15"/>
       <c r="H81" s="15"/>
-      <c r="I81" s="18"/>
-      <c r="J81" s="18"/>
+      <c r="I81" s="20"/>
+      <c r="J81" s="20"/>
     </row>
     <row r="82" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
-      <c r="J82" s="19"/>
+      <c r="B82" s="16"/>
+      <c r="C82" s="16"/>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
     </row>
     <row r="83" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
@@ -2373,7 +2362,7 @@
       <c r="F83" s="17"/>
       <c r="G83" s="17"/>
       <c r="H83" s="17"/>
-      <c r="I83" s="18"/>
+      <c r="I83" s="20"/>
       <c r="J83" s="17"/>
     </row>
     <row r="84" spans="1:10" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2389,18 +2378,18 @@
       <c r="J84" s="15"/>
     </row>
     <row r="85" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
+      <c r="A85" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="19"/>
-      <c r="G85" s="19"/>
-      <c r="H85" s="19"/>
-      <c r="I85" s="19"/>
-      <c r="J85" s="19"/>
+      <c r="B85" s="16"/>
+      <c r="C85" s="16"/>
+      <c r="D85" s="16"/>
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="16"/>
+      <c r="H85" s="16"/>
+      <c r="I85" s="16"/>
+      <c r="J85" s="16"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
@@ -2408,13 +2397,13 @@
       </c>
       <c r="B86" s="17"/>
       <c r="C86" s="17"/>
-      <c r="D86" s="45"/>
-      <c r="E86" s="46"/>
-      <c r="F86" s="46"/>
-      <c r="G86" s="46"/>
-      <c r="H86" s="46"/>
-      <c r="I86" s="46"/>
-      <c r="J86" s="46"/>
+      <c r="D86" s="21"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+      <c r="G86" s="22"/>
+      <c r="H86" s="22"/>
+      <c r="I86" s="22"/>
+      <c r="J86" s="22"/>
     </row>
     <row r="87" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="15"/>
@@ -2429,80 +2418,42 @@
       <c r="J87" s="15"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A88" s="19" t="s">
+      <c r="A88" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-      <c r="F88" s="19"/>
-      <c r="G88" s="19"/>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
-      <c r="J88" s="19"/>
+      <c r="B88" s="16"/>
+      <c r="C88" s="16"/>
+      <c r="D88" s="16"/>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
+      <c r="J88" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A68:J68"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="A70:J70"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="E71:J71"/>
-    <mergeCell ref="A72:J72"/>
-    <mergeCell ref="A63:J63"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="D64:J64"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="C67:J67"/>
-    <mergeCell ref="A88:J88"/>
-    <mergeCell ref="A79:J79"/>
-    <mergeCell ref="A80:H80"/>
-    <mergeCell ref="I80:J80"/>
-    <mergeCell ref="A81:J81"/>
-    <mergeCell ref="A82:J82"/>
-    <mergeCell ref="A83:H83"/>
-    <mergeCell ref="I83:J83"/>
-    <mergeCell ref="A73:J73"/>
-    <mergeCell ref="A74:E74"/>
-    <mergeCell ref="F74:J74"/>
-    <mergeCell ref="A75:J75"/>
-    <mergeCell ref="A76:J76"/>
-    <mergeCell ref="A78:J78"/>
-    <mergeCell ref="A84:J84"/>
-    <mergeCell ref="A85:J85"/>
-    <mergeCell ref="A86:C86"/>
-    <mergeCell ref="D86:J86"/>
-    <mergeCell ref="A87:J87"/>
-    <mergeCell ref="F61:J61"/>
-    <mergeCell ref="A62:J62"/>
-    <mergeCell ref="A53:J53"/>
-    <mergeCell ref="A57:J57"/>
-    <mergeCell ref="A58:D58"/>
-    <mergeCell ref="E58:J58"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="A50:J50"/>
-    <mergeCell ref="A51:J51"/>
-    <mergeCell ref="A52:J52"/>
-    <mergeCell ref="A59:J59"/>
-    <mergeCell ref="A60:J60"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="E54:H54"/>
-    <mergeCell ref="E56:H56"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="F44:J44"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="A46:J46"/>
-    <mergeCell ref="A47:D47"/>
-    <mergeCell ref="E47:J47"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:F41"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="A42:J42"/>
-    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A14:J14"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A8:J8"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="A9:J9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A16:J16"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="E38:J38"/>
     <mergeCell ref="A30:J30"/>
@@ -2527,27 +2478,65 @@
     <mergeCell ref="A22:J22"/>
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="F23:J23"/>
-    <mergeCell ref="A24:J24"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A14:J14"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A8:J8"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:J7"/>
-    <mergeCell ref="A9:J9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="F44:J44"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A47:D47"/>
+    <mergeCell ref="E47:J47"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:F41"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="A42:J42"/>
+    <mergeCell ref="A43:J43"/>
+    <mergeCell ref="F61:J61"/>
+    <mergeCell ref="A62:J62"/>
+    <mergeCell ref="A53:J53"/>
+    <mergeCell ref="A57:J57"/>
+    <mergeCell ref="A58:D58"/>
+    <mergeCell ref="E58:J58"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A50:J50"/>
+    <mergeCell ref="A51:J51"/>
+    <mergeCell ref="A52:J52"/>
+    <mergeCell ref="A59:J59"/>
+    <mergeCell ref="A60:J60"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="E54:H54"/>
+    <mergeCell ref="E56:H56"/>
+    <mergeCell ref="A88:J88"/>
+    <mergeCell ref="A79:J79"/>
+    <mergeCell ref="A80:H80"/>
+    <mergeCell ref="I80:J80"/>
+    <mergeCell ref="A81:J81"/>
+    <mergeCell ref="A82:J82"/>
+    <mergeCell ref="A83:H83"/>
+    <mergeCell ref="I83:J83"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="A74:E74"/>
+    <mergeCell ref="F74:J74"/>
+    <mergeCell ref="A75:J75"/>
+    <mergeCell ref="A76:J76"/>
+    <mergeCell ref="A78:J78"/>
+    <mergeCell ref="A84:J84"/>
+    <mergeCell ref="A85:J85"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="D86:J86"/>
+    <mergeCell ref="A87:J87"/>
+    <mergeCell ref="A68:J68"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="A70:J70"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="E71:J71"/>
+    <mergeCell ref="A72:J72"/>
+    <mergeCell ref="A63:J63"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="D64:J64"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="C67:J67"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.59055118110236227" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="85" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix borders and add multiline
</commit_message>
<xml_diff>
--- a/plugin/act_builder_lib/actOSR.xlsx
+++ b/plugin/act_builder_lib/actOSR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danek\Documents\GitHub\builders_act_maker\plugin\act_builder_lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0C29F1-365E-4C14-B2E6-2304E5B9C446}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BFE9ED-2CE4-40CF-B046-A29DDD45C0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="791" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,7 +695,7 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -749,76 +749,67 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="12" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="12" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1173,8 +1164,8 @@
   </sheetPr>
   <dimension ref="A1:BE88"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1230,187 +1221,187 @@
       <c r="J3" s="13"/>
     </row>
     <row r="4" spans="1:10" s="9" customFormat="1" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
     </row>
     <row r="6" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-      <c r="J7" s="31"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
     </row>
     <row r="8" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="37"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
     </row>
     <row r="10" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
-      <c r="J10" s="32"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" s="4" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
     </row>
     <row r="14" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="33"/>
-      <c r="G14" s="33"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="33"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" spans="1:10" s="9" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="33" t="s">
+      <c r="A15" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="33"/>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-      <c r="J15" s="33"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="29"/>
-      <c r="C16" s="29"/>
-      <c r="D16" s="29"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="29"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="29"/>
-      <c r="J16" s="29"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
     </row>
     <row r="17" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1434,12 +1425,12 @@
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
     </row>
     <row r="21" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
@@ -1454,18 +1445,18 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:12" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
+      <c r="A22" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
-      <c r="J22" s="21"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
     </row>
     <row r="23" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -1482,16 +1473,16 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
+      <c r="A24" s="22"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
@@ -1535,18 +1526,18 @@
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="1:12" s="4" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="21"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="21"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
-      <c r="J28" s="21"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
     </row>
     <row r="29" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
@@ -1564,30 +1555,30 @@
       <c r="L29" s="8"/>
     </row>
     <row r="30" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
     </row>
     <row r="31" spans="1:12" s="4" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="21"/>
-      <c r="F31" s="21"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
-      <c r="J31" s="21"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
     </row>
     <row r="32" spans="1:12" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
@@ -1604,70 +1595,70 @@
       <c r="J32" s="15"/>
     </row>
     <row r="33" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
+      <c r="G33" s="24"/>
+      <c r="H33" s="24"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="24"/>
     </row>
     <row r="34" spans="1:57" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
-      <c r="J34" s="21"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
     </row>
     <row r="35" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="32" t="s">
+      <c r="A35" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="32"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="32"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
     </row>
     <row r="36" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="25" t="s">
+      <c r="A37" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
     </row>
     <row r="38" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
@@ -1688,14 +1679,14 @@
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="F39" s="23"/>
-      <c r="G39" s="23"/>
-      <c r="H39" s="23"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="23"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="38"/>
     </row>
     <row r="40" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="14" t="s">
@@ -1715,36 +1706,36 @@
       <c r="D41" s="14"/>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
     </row>
     <row r="43" spans="1:57" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="25" t="s">
+      <c r="A43" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
     </row>
     <row r="44" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
@@ -1754,11 +1745,11 @@
       <c r="C44" s="14"/>
       <c r="D44" s="14"/>
       <c r="E44" s="14"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
@@ -1773,18 +1764,18 @@
       <c r="J45" s="12"/>
     </row>
     <row r="46" spans="1:57" s="4" customFormat="1" ht="26.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="B46" s="22"/>
-      <c r="C46" s="22"/>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
+      <c r="B46" s="37"/>
+      <c r="C46" s="37"/>
+      <c r="D46" s="37"/>
+      <c r="E46" s="37"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
+      <c r="J46" s="37"/>
     </row>
     <row r="47" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
@@ -1801,16 +1792,16 @@
       <c r="J47" s="17"/>
     </row>
     <row r="48" spans="1:57" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="41"/>
-      <c r="B48" s="41"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
-      <c r="F48" s="42"/>
-      <c r="G48" s="42"/>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
+      <c r="A48" s="35"/>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
@@ -1860,18 +1851,18 @@
       <c r="BE48" s="6"/>
     </row>
     <row r="49" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="25" t="s">
+      <c r="A49" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
     </row>
     <row r="50" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
@@ -1914,16 +1905,16 @@
       <c r="J52" s="13"/>
     </row>
     <row r="53" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="39"/>
-      <c r="B53" s="39"/>
-      <c r="C53" s="39"/>
-      <c r="D53" s="39"/>
-      <c r="E53" s="39"/>
-      <c r="F53" s="39"/>
-      <c r="G53" s="39"/>
-      <c r="H53" s="39"/>
-      <c r="I53" s="39"/>
-      <c r="J53" s="39"/>
+      <c r="A53" s="33"/>
+      <c r="B53" s="33"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="33"/>
+      <c r="E53" s="33"/>
+      <c r="F53" s="33"/>
+      <c r="G53" s="33"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="33"/>
+      <c r="J53" s="33"/>
     </row>
     <row r="54" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
@@ -1933,10 +1924,10 @@
         <v>12</v>
       </c>
       <c r="D54" s="10"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="20"/>
-      <c r="H54" s="20"/>
+      <c r="E54" s="19"/>
+      <c r="F54" s="19"/>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D55" s="2"/>
@@ -1948,10 +1939,10 @@
         <v>13</v>
       </c>
       <c r="D56" s="10"/>
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="20"/>
-      <c r="H56" s="20"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
     </row>
     <row r="57" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16"/>
@@ -1972,24 +1963,24 @@
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="40"/>
-      <c r="G58" s="40"/>
-      <c r="H58" s="40"/>
-      <c r="I58" s="40"/>
-      <c r="J58" s="40"/>
+      <c r="E58" s="17"/>
+      <c r="F58" s="34"/>
+      <c r="G58" s="34"/>
+      <c r="H58" s="34"/>
+      <c r="I58" s="34"/>
+      <c r="J58" s="34"/>
     </row>
     <row r="59" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="19"/>
-      <c r="B59" s="19"/>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="19"/>
-      <c r="F59" s="19"/>
-      <c r="G59" s="19"/>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
+      <c r="A59" s="12"/>
+      <c r="B59" s="12"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
+      <c r="H59" s="12"/>
+      <c r="I59" s="12"/>
+      <c r="J59" s="12"/>
     </row>
     <row r="60" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="13" t="s">
@@ -2013,11 +2004,11 @@
       <c r="C61" s="14"/>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
-      <c r="I61" s="12"/>
-      <c r="J61" s="12"/>
+      <c r="F61" s="17"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17"/>
     </row>
     <row r="62" spans="1:10" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="12"/>
@@ -2372,19 +2363,25 @@
     </row>
   </sheetData>
   <mergeCells count="97">
-    <mergeCell ref="A35:J35"/>
-    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="F44:J44"/>
+    <mergeCell ref="A45:J45"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:F41"/>
     <mergeCell ref="A47:D47"/>
     <mergeCell ref="E47:J47"/>
     <mergeCell ref="F61:J61"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A50:J50"/>
     <mergeCell ref="A62:J62"/>
     <mergeCell ref="A53:J53"/>
     <mergeCell ref="A57:J57"/>
     <mergeCell ref="A58:D58"/>
     <mergeCell ref="E58:J58"/>
-    <mergeCell ref="A48:J48"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="A50:J50"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A14:J14"/>
@@ -2401,6 +2398,7 @@
     <mergeCell ref="A4:J4"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A10:J10"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="E38:J38"/>
@@ -2417,14 +2415,6 @@
     <mergeCell ref="A27:J27"/>
     <mergeCell ref="A28:J28"/>
     <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A44:E44"/>
-    <mergeCell ref="F44:J44"/>
-    <mergeCell ref="A45:J45"/>
-    <mergeCell ref="A46:J46"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="A40:E40"/>
-    <mergeCell ref="A41:F41"/>
     <mergeCell ref="G41:J41"/>
     <mergeCell ref="A42:J42"/>
     <mergeCell ref="A43:J43"/>
@@ -2433,6 +2423,7 @@
     <mergeCell ref="A26:J26"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="A32:J32"/>
+    <mergeCell ref="A35:J35"/>
     <mergeCell ref="A51:J51"/>
     <mergeCell ref="A52:J52"/>
     <mergeCell ref="A59:J59"/>

</xml_diff>